<commit_message>
Ajuste final 18_08 01
</commit_message>
<xml_diff>
--- a/Pontos das respostas.xlsx
+++ b/Pontos das respostas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_LC\painel-eduser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA62EB0E-02B9-4D1F-8270-1EA352A0069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F80DD4A-5717-42C0-8EF5-191720105DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{BF6C3C50-8D9E-4593-9687-54073694C3D5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF6C3C50-8D9E-4593-9687-54073694C3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Supabase Snippet Question Optio" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,8 +552,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -731,18 +739,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -906,22 +902,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1297,1982 +1287,1863 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A68A5C4-5C34-4DD1-969D-38DDC1729668}">
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="70.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="b">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="b">
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="b">
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="b">
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="b">
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="1" t="b">
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="1" t="b">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39">
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="1" t="b">
+      <c r="B40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41">
+      <c r="B41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="1" t="b">
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B45" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45">
+      <c r="B45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46">
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="1" t="b">
+      <c r="B47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B48" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="1" t="b">
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="1" t="b">
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B51" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51">
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="1" t="b">
+      <c r="B52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="B53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B54" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="D54" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="3"/>
-      <c r="H57" s="6"/>
-    </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="3" t="s">
+      <c r="B58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="1">
         <v>2</v>
       </c>
-      <c r="H58" s="6"/>
-    </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="3" t="s">
+      <c r="B59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="4">
-        <v>1</v>
-      </c>
-      <c r="E59" s="2">
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
         <v>2</v>
       </c>
-      <c r="F59" s="2">
-        <v>1</v>
-      </c>
-      <c r="H59" s="6"/>
-    </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="3"/>
-      <c r="H60" s="6"/>
-    </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="3" t="s">
+      <c r="B61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D61" s="4">
-        <v>1</v>
-      </c>
-      <c r="H61" s="6"/>
-    </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="B62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="4">
-        <v>1</v>
-      </c>
-      <c r="H62" s="6"/>
-    </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="3" t="s">
+      <c r="B63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="4">
-        <v>1</v>
-      </c>
-      <c r="H63" s="6"/>
-    </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="B64" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D64" s="4">
-        <v>1</v>
-      </c>
-      <c r="H64" s="6"/>
-    </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="3" t="s">
+      <c r="B65" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="4">
-        <v>1</v>
-      </c>
-      <c r="H65" s="6"/>
-    </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+      <c r="D65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="3" t="s">
+      <c r="B66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="4">
-        <v>1</v>
-      </c>
-      <c r="H66" s="6"/>
-    </row>
-    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="D66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="3" t="s">
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D67" s="1">
         <v>2</v>
       </c>
-      <c r="H67" s="6"/>
-    </row>
-    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="3" t="s">
+      <c r="B68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D68" s="1">
         <v>2</v>
       </c>
-      <c r="H68" s="6"/>
-    </row>
-    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="3" t="s">
+      <c r="B69" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D69" s="4">
-        <v>5</v>
-      </c>
-      <c r="H69" s="6"/>
-    </row>
-    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="D69" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="3" t="s">
+      <c r="B70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D70" s="1">
         <v>6</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="1">
         <v>6</v>
       </c>
-      <c r="F70" s="2">
-        <v>1</v>
-      </c>
-      <c r="H70" s="6"/>
-    </row>
-    <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="3"/>
-      <c r="H71" s="6"/>
-    </row>
-    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="F70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="3" t="s">
+      <c r="B72" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="4">
-        <v>5</v>
-      </c>
-      <c r="H72" s="6"/>
-    </row>
-    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="D72" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="3" t="s">
+      <c r="B73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D73" s="1">
         <v>6</v>
       </c>
-      <c r="H73" s="6"/>
-    </row>
-    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="3" t="s">
+      <c r="B74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D74" s="1">
         <v>7</v>
       </c>
-      <c r="H74" s="6"/>
-    </row>
-    <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="3" t="s">
+      <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D75" s="1">
         <v>8</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="1">
         <v>8</v>
       </c>
-      <c r="F75" s="2">
-        <v>5</v>
-      </c>
-      <c r="H75" s="6"/>
-    </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="3"/>
-      <c r="H76" s="6"/>
-    </row>
-    <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+      <c r="F75" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="3" t="s">
+      <c r="B77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D77" s="1">
         <v>2</v>
       </c>
-      <c r="H77" s="6"/>
-    </row>
-    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="3" t="s">
+      <c r="B78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D78" s="1">
         <v>8</v>
       </c>
-      <c r="H78" s="6"/>
-    </row>
-    <row r="79" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="3" t="s">
+      <c r="B79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D79" s="1">
         <v>12</v>
       </c>
-      <c r="H79" s="6"/>
-    </row>
-    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="3" t="s">
+      <c r="B80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D80" s="1">
         <v>12</v>
       </c>
-      <c r="H80" s="6"/>
-    </row>
-    <row r="81" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="3" t="s">
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D81" s="1">
         <v>13</v>
       </c>
-      <c r="H81" s="6"/>
-    </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="3" t="s">
+      <c r="B82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D82" s="1">
         <v>14</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="1">
         <v>14</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82" s="1">
         <v>2</v>
       </c>
-      <c r="H82" s="6"/>
-    </row>
-    <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C83" s="3"/>
-      <c r="H83" s="6"/>
-    </row>
-    <row r="84" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C84" s="3" t="s">
+      <c r="B84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D84" s="1">
         <v>2</v>
       </c>
-      <c r="H84" s="6"/>
-    </row>
-    <row r="85" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="3" t="s">
+      <c r="B85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D85" s="1">
         <v>4</v>
       </c>
-      <c r="H85" s="6"/>
-    </row>
-    <row r="86" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="3" t="s">
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D86" s="1">
         <v>8</v>
       </c>
-      <c r="H86" s="6"/>
-    </row>
-    <row r="87" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="3" t="s">
+      <c r="B87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D87" s="1">
         <v>11</v>
       </c>
-      <c r="H87" s="6"/>
-    </row>
-    <row r="88" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="3" t="s">
+      <c r="B88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D88" s="1">
         <v>12</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="1">
         <v>12</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F88" s="1">
         <v>2</v>
       </c>
-      <c r="H88" s="6"/>
-    </row>
-    <row r="89" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C89" s="3"/>
-      <c r="H89" s="6"/>
-    </row>
-    <row r="90" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="3" t="s">
+      <c r="B90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D90" s="2">
-        <v>1</v>
-      </c>
-      <c r="H90" s="6"/>
-    </row>
-    <row r="91" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="D90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="3" t="s">
+      <c r="B91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="1">
         <v>4</v>
       </c>
-      <c r="H91" s="6"/>
-    </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="3" t="s">
+      <c r="B92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D92" s="2">
-        <v>5</v>
-      </c>
-      <c r="H92" s="6"/>
-    </row>
-    <row r="93" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
+      <c r="D92" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="3" t="s">
+      <c r="B93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="1">
         <v>7</v>
       </c>
-      <c r="H93" s="6"/>
-    </row>
-    <row r="94" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C94" s="3" t="s">
+      <c r="B94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="1">
         <v>7</v>
       </c>
-      <c r="H94" s="6"/>
-    </row>
-    <row r="95" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="3" t="s">
+      <c r="B95" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D95" s="1">
         <v>12</v>
       </c>
-      <c r="H95" s="6"/>
-    </row>
-    <row r="96" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="3" t="s">
+      <c r="B96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D96" s="1">
         <v>15</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96" s="1">
         <v>15</v>
       </c>
-      <c r="F96" s="2">
-        <v>1</v>
-      </c>
-      <c r="H96" s="6"/>
-    </row>
-    <row r="97" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C97" s="3"/>
-      <c r="H97" s="6"/>
-    </row>
-    <row r="98" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
+      <c r="F96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" s="3" t="s">
+      <c r="B98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="H98" s="6"/>
-    </row>
-    <row r="99" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
+      <c r="D98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="3" t="s">
+      <c r="B99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99" s="1">
         <v>2</v>
       </c>
-      <c r="H99" s="6"/>
-    </row>
-    <row r="100" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="3" t="s">
+      <c r="B100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100" s="1">
         <v>3</v>
       </c>
-      <c r="H100" s="6"/>
-    </row>
-    <row r="101" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="3" t="s">
+      <c r="B101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="1">
         <v>4</v>
       </c>
-      <c r="H101" s="6"/>
-    </row>
-    <row r="102" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="3" t="s">
+      <c r="B102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D102" s="2">
-        <v>5</v>
-      </c>
-      <c r="H102" s="6"/>
-    </row>
-    <row r="103" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
+      <c r="D102" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="3" t="s">
+      <c r="B103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D103" s="2">
-        <v>5</v>
-      </c>
-      <c r="H103" s="6"/>
-    </row>
-    <row r="104" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
+      <c r="D103" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="3" t="s">
+      <c r="B104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D104" s="2">
-        <v>5</v>
-      </c>
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+      <c r="D104" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="3" t="s">
+      <c r="B105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D105" s="2">
-        <v>5</v>
-      </c>
-      <c r="H105" s="6"/>
-    </row>
-    <row r="106" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
+      <c r="D105" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="3" t="s">
+      <c r="B106" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D106" s="2">
-        <v>5</v>
-      </c>
-      <c r="H106" s="6"/>
-    </row>
-    <row r="107" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+      <c r="D106" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="3" t="s">
+      <c r="B107" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D107" s="2">
-        <v>5</v>
-      </c>
-      <c r="H107" s="6"/>
-    </row>
-    <row r="108" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
+      <c r="D107" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" s="3" t="s">
+      <c r="B108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D108" s="1">
         <v>6</v>
       </c>
-      <c r="H108" s="6"/>
-    </row>
-    <row r="109" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="3" t="s">
+      <c r="B109" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D109" s="1">
         <v>6</v>
       </c>
-      <c r="H109" s="6"/>
-    </row>
-    <row r="110" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="3" t="s">
+      <c r="B110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D110" s="2">
+      <c r="D110" s="1">
         <v>6</v>
       </c>
-      <c r="H110" s="6"/>
-    </row>
-    <row r="111" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="3" t="s">
+      <c r="B111" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111" s="1">
         <v>6</v>
       </c>
-      <c r="H111" s="6"/>
-    </row>
-    <row r="112" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="3" t="s">
+      <c r="B112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112" s="1">
         <v>6</v>
       </c>
-      <c r="H112" s="6"/>
-    </row>
-    <row r="113" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" s="3" t="s">
+      <c r="B113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D113" s="1">
         <v>7</v>
       </c>
-      <c r="H113" s="6"/>
-    </row>
-    <row r="114" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" s="3" t="s">
+      <c r="B114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114" s="1">
         <v>7</v>
       </c>
-      <c r="H114" s="6"/>
-    </row>
-    <row r="115" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" s="3" t="s">
+      <c r="B115" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D115" s="2">
+      <c r="D115" s="1">
         <v>7</v>
       </c>
-      <c r="H115" s="6"/>
-    </row>
-    <row r="116" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C116" s="3" t="s">
+      <c r="B116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116" s="1">
         <v>7</v>
       </c>
-      <c r="H116" s="6"/>
-    </row>
-    <row r="117" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="3" t="s">
+      <c r="B117" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D117" s="1">
         <v>7</v>
       </c>
-      <c r="H117" s="6"/>
-    </row>
-    <row r="118" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C118" s="3" t="s">
+      <c r="B118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D118" s="2">
+      <c r="D118" s="1">
         <v>7</v>
       </c>
-      <c r="H118" s="6"/>
-    </row>
-    <row r="119" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C119" s="3" t="s">
+      <c r="B119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D119" s="2">
+      <c r="D119" s="1">
         <v>8</v>
       </c>
-      <c r="H119" s="6"/>
-    </row>
-    <row r="120" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C120" s="3" t="s">
+      <c r="B120" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D120" s="2">
+      <c r="D120" s="1">
         <v>9</v>
       </c>
-      <c r="H120" s="6"/>
-    </row>
-    <row r="121" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" s="3" t="s">
+      <c r="B121" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D121" s="2">
+      <c r="D121" s="1">
         <v>9</v>
       </c>
-      <c r="H121" s="6"/>
-    </row>
-    <row r="122" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" s="3" t="s">
+      <c r="B122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D122" s="2">
+      <c r="D122" s="1">
         <v>10</v>
       </c>
-      <c r="H122" s="6"/>
-    </row>
-    <row r="123" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C123" s="3" t="s">
+      <c r="B123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D123" s="1">
         <v>17</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E123" s="1">
         <v>17</v>
       </c>
-      <c r="F123" s="2">
-        <v>1</v>
-      </c>
-      <c r="H123" s="6"/>
-    </row>
-    <row r="124" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
+      <c r="F123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C124" s="3" t="s">
+      <c r="B124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D124" s="1">
         <v>17</v>
       </c>
-      <c r="H124" s="6"/>
-    </row>
-    <row r="125" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C125" s="3"/>
-      <c r="H125" s="6"/>
-    </row>
-    <row r="126" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" s="3" t="s">
+      <c r="B126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D126" s="2">
+      <c r="D126" s="1">
         <v>4</v>
       </c>
-      <c r="H126" s="6"/>
-    </row>
-    <row r="127" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C127" s="3" t="s">
+      <c r="B127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D127" s="2">
+      <c r="D127" s="1">
         <v>4</v>
       </c>
-      <c r="H127" s="6"/>
-    </row>
-    <row r="128" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C128" s="3" t="s">
+      <c r="B128" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D128" s="2">
+      <c r="D128" s="1">
         <v>8</v>
       </c>
-      <c r="H128" s="6"/>
-    </row>
-    <row r="129" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C129" s="3" t="s">
+      <c r="B129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D129" s="2">
+      <c r="D129" s="1">
         <v>9</v>
       </c>
-      <c r="H129" s="6"/>
-    </row>
-    <row r="130" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C130" s="3" t="s">
+      <c r="B130" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D130" s="2">
+      <c r="D130" s="1">
         <v>9</v>
       </c>
-      <c r="H130" s="6"/>
-    </row>
-    <row r="131" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C131" s="3" t="s">
+      <c r="B131" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D131" s="2">
+      <c r="D131" s="1">
         <v>11</v>
       </c>
-      <c r="H131" s="6"/>
-    </row>
-    <row r="132" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C132" s="3" t="s">
+      <c r="B132" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D132" s="2">
+      <c r="D132" s="1">
         <v>12</v>
       </c>
-      <c r="E132" s="2">
+      <c r="E132" s="1">
         <v>12</v>
       </c>
-      <c r="F132" s="2">
+      <c r="F132" s="1">
         <v>4</v>
       </c>
-      <c r="H132" s="6"/>
-    </row>
-    <row r="133" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C133" s="3"/>
-      <c r="H133" s="6"/>
-    </row>
-    <row r="134" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C134" s="3" t="s">
+      <c r="B134" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D134" s="1">
         <v>2</v>
       </c>
-      <c r="H134" s="6"/>
-    </row>
-    <row r="135" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C135" s="3" t="s">
+      <c r="B135" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D135" s="1">
         <v>10</v>
       </c>
-      <c r="E135" s="2">
+      <c r="E135" s="1">
         <v>10</v>
       </c>
-      <c r="F135" s="2">
+      <c r="F135" s="1">
         <v>2</v>
       </c>
-      <c r="H135" s="6"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E137">
+      <c r="E137" s="1">
         <f>SUM(E1:E136)</f>
         <v>96</v>
       </c>
-      <c r="F137">
-        <f t="shared" ref="E137:F137" si="0">SUM(F1:F136)</f>
+      <c r="F137" s="1">
+        <f t="shared" ref="F137" si="0">SUM(F1:F136)</f>
         <v>19</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I138">
-        <v>1</v>
-      </c>
-      <c r="J138">
-        <v>34</v>
-      </c>
+      <c r="I138" s="4"/>
+      <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I139">
-        <v>35</v>
-      </c>
-      <c r="J139">
-        <v>49</v>
-      </c>
+      <c r="I139" s="4"/>
+      <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I140">
-        <v>50</v>
-      </c>
-      <c r="J140">
-        <v>64</v>
-      </c>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I141">
-        <v>65</v>
-      </c>
-      <c r="J141">
-        <v>79</v>
-      </c>
+      <c r="F141" s="4"/>
+      <c r="I141" s="4"/>
+      <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I142">
-        <v>80</v>
-      </c>
-      <c r="J142">
-        <v>100</v>
-      </c>
+      <c r="I142" s="4"/>
+      <c r="J142" s="4"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I143" s="4"/>
+      <c r="J143" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D153">

</xml_diff>